<commit_message>
add more test files
</commit_message>
<xml_diff>
--- a/Saved_Lists/Inventory.xlsx
+++ b/Saved_Lists/Inventory.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,150 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>311-9.76KCRCT-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>RC0805FR-079K76L</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>RES 9.76K OHM 1% 1/8W 0805</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>541-4138-1-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CRCW08054K99FKEAC</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>RES 4.99K OHM 1% 1/8W 0805</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.092</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>311-1.00CRCT-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>RC0805FR-071RL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>RES 1 OHM 1% 1/8W 0805</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>311-1.00KCRCT-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>RC0805FR-071KL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>RES 1K OHM 1% 1/8W 0805</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.062</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RNCP0805FTD10K0CT-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RNCP0805FTD10K0</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>RES 10K OHM 1% 1/4W 0805</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.0439</v>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2019-RK73H2ATTD2200FCT-ND</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RK73H2ATTD2200F</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>RES 220 OHM 1% 1/4W 0805</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.0253</v>
+      </c>
+      <c r="F7" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +674,78 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>732-4982-1-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>150080BS75000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>LED BLUE CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>732-4986-1-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>150080VS75000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>LED GREEN CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>732-4985-1-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>150080SS75000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>LED RED CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -581,6 +797,54 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1738-1041-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DFR0299</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DFPLAYER - A MINI MP3 PLAYER</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>8.19</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>433-1259-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SP-3005Y</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SPEAKER 8OHM 1W TOP PORT 87DB</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>2.48</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -645,7 +909,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,6 +947,30 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1738-1038-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DFR0229</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MICROSD CARD MODULE FOR ARDUINO</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>7.16</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +1137,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -887,6 +1175,30 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DKS-PCB-RULER-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>DKS-PCB-RULER-12INCH</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PCB LAYOUT REFERENCE RULER 12"</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -900,7 +1212,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -940,165 +1252,116 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>399-C0805C103K1RAC7800CT-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>C0805C103K1RAC7800</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CAP CER 10000PF 100V X7R 0805</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>10NF OR 0.01UF</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>399-C0805C104K5RAC7800CT-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>C0805C104K5RAC7800</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CAP CER 0.1UF 50V X7R 0805</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>100NF OR 0.1UF</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>P16560CT-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>35SVPF22M</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CAP ALUM POLY 22UF 20% 35V SMD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>399-A768MS107M1HLAE024CT-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A768MS107M1HLAE024</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CAP ALUM POLY 100UF 20% 50V SMD</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Digi-Key Part #</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Manufacturer Part Number</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Customer Reference</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Digi-Key Part #</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Manufacturer Part Number</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Customer Reference</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Digi-Key Part #</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Manufacturer Part Number</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Customer Reference</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1147,6 +1410,351 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>PCD2434CT-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ETQ-P5M330YFC</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FIXED IND 33UH 5A 75.4 MOHM SMD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1514-PN2222APBFREE-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PN2222A PBFREE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TRANS NPN 40V 0.8A TO92-3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>PZT2222AT1GOSCT-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PZT2222AT1G</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TRANS NPN 40V 0.6A SOT223</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>497-5236-1-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2STD1665T4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TRANS NPN 65V 6A DPAK</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SB5100DICT-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>SB5100-T</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DIODE SCHOTTKY 100V 5A DO201AD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.899</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SK54B-LTPMSCT-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SK54B-LTP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DIODE SCHOTTKY 40V 5A DO214AA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>FDLL4148CT-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FDLL4148</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>DIODE GEN PURP 100V 200MA SOD80</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1655-DSS14UCT-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DSS14U</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DIODE SCHOTTKY 40V 1A SOD123FL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.263</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>788-1091-ND</t>
         </is>
       </c>
@@ -1166,6 +1774,126 @@
       </c>
       <c r="F2" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>296-1414-5-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>RC4558P</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>296-NE555P-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>NE555P</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>IC OSC SINGLE TIMER 100KHZ 8-DIP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>296-43515-5-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LM2679S-ADJ/NOPB</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IC REG BUCK ADJ 5A TO263-7</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>11.01</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>296-14118-5-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CD4056BE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>IC DRVR 7 SEGMENT 1 DIGIT 16DIP</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>296-31512-1-ND</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CD4056BM96</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>IC DRVR 7 SEGMENT 1 DIGIT 16SOIC</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1179,7 +1907,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1217,6 +1945,78 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A98333-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>282834-2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TERM BLK 2P SIDE ENT 2.54MM PCB</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ED10563-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OSTVN04A150</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TERM BLK 4P SIDE ENT 2.54MM PCB</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2092-SX1100-B-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>SX1100-B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CONN SHUNT BLACK OPEN TOP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1230,7 +2030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1268,6 +2068,30 @@
         <is>
           <t>Quantity</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1830-1161-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>INND-TS56RCB</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>DISPLAY 7SEG 0.56" SGL RED 10DIP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +2105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1321,6 +2145,78 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CKN12304-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PTS636 SP43 LFS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TACT 6.0 X 3.5, 4.3 MM H, 320GF,</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.133</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CKN12222-1-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>PTS526 SMG15 SMTR2 LFS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TACT 5.2 X 5.2, 1.5 MM H, 160GF,</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.207</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CKN12317-1-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PTS636 SM43J SMTR LFS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TACT 6.0 X 3.5, 4.3 MM H, 180GF,</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
syncing inventory & orders
</commit_message>
<xml_diff>
--- a/Saved_Lists/Inventory.xlsx
+++ b/Saved_Lists/Inventory.xlsx
@@ -14,17 +14,21 @@
     <sheet name="Diodes" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Regulator" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="ICs" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Connectors" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Displays" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Buttons, Switches" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="LEDs" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Audio" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Potentiometer" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Modules" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Fans" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="ACDC Converters" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="AC Transformer" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Other" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Logic Gates" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Connectors" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Displays" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Buttons, Switches" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="LEDs" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Audio" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Potentiometer" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Modules" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Fans" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="ACDC Converters" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="AC Transformer" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Resonators, Crystals" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Encoders" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Relay" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Other" sheetId="22" state="visible" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -485,238 +489,238 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>311-9.76KCRCT-ND</t>
+          <t>RMCF0805JG470RCT-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>RC0805FR-079K76L</t>
+          <t>RMCF0805JG470R</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>RES 9.76K OHM 1% 1/8W 0805</t>
+          <t>RES 470 OHM 5% 1/8W 0805</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.062</v>
+        <v>0.0126</v>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>541-4138-1-ND</t>
+          <t>RMCF0805JT390RCT-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CRCW08054K99FKEAC</t>
+          <t>RMCF0805JT390R</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RES 4.99K OHM 1% 1/8W 0805</t>
+          <t>RES 390 OHM 5% 1/8W 0805</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.092</v>
+        <v>0.0126</v>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>311-1.00CRCT-ND</t>
+          <t>2019-RK73B2ATTD512JCT-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>RC0805FR-071RL</t>
+          <t>RK73B2ATTD512J</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>RES 1 OHM 1% 1/8W 0805</t>
+          <t>RES 5.1K OHM 5% 1/4W 0805</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.122</v>
+        <v>0.0185</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>311-1.00KCRCT-ND</t>
+          <t>90.9KXBK-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>RC0805FR-071KL</t>
+          <t>MFR-25FBF52-90K9</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>RES 1K OHM 1% 1/8W 0805</t>
+          <t>RES 90.9K OHM 1% 1/4W AXIAL</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.062</v>
+        <v>0.0804</v>
       </c>
       <c r="F5" t="n">
-        <v>120</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RNCP0805FTD10K0CT-ND</t>
+          <t>311-9.76KCRCT-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RNCP0805FTD10K0</t>
+          <t>RC0805FR-079K76L</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>RES 10K OHM 1% 1/4W 0805</t>
+          <t>RES 9.76K OHM 1% 1/8W 0805</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>0.0439</v>
+        <v>0.062</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2019-RK73H2ATTD2200FCT-ND</t>
+          <t>541-4138-1-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RK73H2ATTD2200F</t>
+          <t>CRCW08054K99FKEAC</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>RES 220 OHM 1% 1/4W 0805</t>
+          <t>RES 4.99K OHM 1% 1/8W 0805</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.0253</v>
+        <v>0.092</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>HS505RF-ND</t>
+          <t>311-1.00CRCT-ND</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>HS50 5R F</t>
+          <t>RC0805FR-071RL</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>RES CHAS MNT 5 OHM 1% 50W</t>
+          <t>RES 1 OHM 1% 1/8W 0805</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>5.86</v>
+        <v>0.122</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>311-1.47KCRCT-ND</t>
+          <t>311-1.00KCRCT-ND</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RC0805FR-071K47L</t>
+          <t>RC0805FR-071KL</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>RES 1.47K OHM 1% 1/8W 0805</t>
+          <t>RES 1K OHM 1% 1/8W 0805</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.0208</v>
+        <v>0.062</v>
       </c>
       <c r="F9" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>90.9KXBK-ND</t>
+          <t>RNCP0805FTD10K0CT-ND</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>MFR-25FBF52-90K9</t>
+          <t>RNCP0805FTD10K0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>RES 90.9K OHM 1% 1/4W AXIAL</t>
+          <t>RES 10K OHM 1% 1/4W 0805</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.0804</v>
+        <v>0.0439</v>
       </c>
       <c r="F10" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RMCF0805JG470RCT-ND</t>
+          <t>2019-RK73H2ATTD2200FCT-ND</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RMCF0805JG470R</t>
+          <t>RK73H2ATTD2200F</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>RES 470 OHM 5% 1/8W 0805</t>
+          <t>RES 220 OHM 1% 1/4W 0805</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.0126</v>
+        <v>0.0253</v>
       </c>
       <c r="F11" t="n">
         <v>100</v>
@@ -725,46 +729,46 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RMCF0805JT390RCT-ND</t>
+          <t>HS505RF-ND</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>RMCF0805JT390R</t>
+          <t>HS50 5R F</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>RES 390 OHM 5% 1/8W 0805</t>
+          <t>RES CHAS MNT 5 OHM 1% 50W</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0126</v>
+        <v>5.86</v>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2019-RK73B2ATTD512JCT-ND</t>
+          <t>311-1.47KCRCT-ND</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>RK73B2ATTD512J</t>
+          <t>RC0805FR-071K47L</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>RES 5.1K OHM 5% 1/4W 0805</t>
+          <t>RES 1.47K OHM 1% 1/8W 0805</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.0185</v>
+        <v>0.0208</v>
       </c>
       <c r="F13" t="n">
         <v>100</v>
@@ -781,7 +785,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -824,73 +828,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CKN12304-ND</t>
+          <t>1830-1161-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PTS636 SP43 LFS</t>
+          <t>INND-TS56RCB</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TACT 6.0 X 3.5, 4.3 MM H, 320GF,</t>
+          <t>DISPLAY 7SEG 0.56" SGL RED 10DIP</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.133</v>
+        <v>1.73</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>CKN12222-1-ND</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>PTS526 SMG15 SMTR2 LFS</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>TACT 5.2 X 5.2, 1.5 MM H, 160GF,</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>0.207</v>
-      </c>
-      <c r="F3" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CKN12317-1-ND</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>PTS636 SM43J SMTR LFS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>TACT 6.0 X 3.5, 4.3 MM H, 180GF,</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>0.211</v>
-      </c>
-      <c r="F4" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -904,7 +860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -947,169 +903,121 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>732-4982-1-ND</t>
+          <t>CT2104MS-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>150080BS75000</t>
+          <t>210-4MS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>LED BLUE CLEAR 0805 SMD</t>
+          <t>SWITCH SLIDE DIP SPST 100MA 20V</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.27</v>
+        <v>0.72</v>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>732-4986-1-ND</t>
+          <t>EG1903-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>150080VS75000</t>
+          <t>EG1218</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>LED GREEN CLEAR 0805 SMD</t>
+          <t>SWITCH SLIDE SPDT 200MA 30V</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.27</v>
+        <v>1.04</v>
       </c>
       <c r="F3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>732-4985-1-ND</t>
+          <t>CKN12304-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>150080SS75000</t>
+          <t>PTS636 SP43 LFS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>LED RED CLEAR 0805 SMD</t>
+          <t>TACT 6.0 X 3.5, 4.3 MM H, 320GF,</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.27</v>
+        <v>0.133</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1125-1191-ND</t>
+          <t>CKN12222-1-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MT5470D-UY</t>
+          <t>PTS526 SMG15 SMTR2 LFS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>LED YELLOW DIFFUSED 5MM OVAL T/H</t>
+          <t>TACT 5.2 X 5.2, 1.5 MM H, 160GF,</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.77</v>
+        <v>0.207</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>C5SMF-RJE-CU14QBB2CT-ND</t>
+          <t>CKN12317-1-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C5SMF-RJE-CU14QBB2</t>
+          <t>PTS636 SM43J SMTR LFS</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>LED RED CLEAR 5MM OVAL T/H</t>
+          <t>TACT 6.0 X 3.5, 4.3 MM H, 180GF,</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>0.29</v>
+        <v>0.211</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>C5SMF-GJE-CX14Q7T2CT-ND</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>C5SMF-GJE-CX14Q7T2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>LED GREEN CLEAR 5MM OVAL T/H</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>1528-1031-ND</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1752</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>EVAL BOARD FOR MAX9744</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>27.96</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1118,6 +1026,201 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>732-4982-1-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>150080BS75000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>LED BLUE CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>732-4986-1-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>150080VS75000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>LED GREEN CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>732-4985-1-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>150080SS75000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>LED RED CLEAR 0805 SMD</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1125-1191-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MT5470D-UY</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>LED YELLOW DIFFUSED 5MM OVAL T/H</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C5SMF-RJE-CU14QBB2CT-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C5SMF-RJE-CU14QBB2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>LED RED CLEAR 5MM OVAL T/H</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>C5SMF-GJE-CX14Q7T2CT-ND</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C5SMF-GJE-CX14Q7T2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>LED GREEN CLEAR 5MM OVAL T/H</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1232,7 +1335,7 @@
         <v>28.74</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1257,57 +1360,6 @@
       </c>
       <c r="F5" t="n">
         <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Digi-Key Part #</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Manufacturer Part Number</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Customer Reference</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unit Price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Quantity</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -1364,25 +1416,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1738-1038-ND</t>
+          <t>PTV09A-4020F-B103-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DFR0229</t>
+          <t>PTV09A-4020F-B103</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MICROSD CARD MODULE FOR ARDUINO</t>
+          <t>POT 10K OHM 1/20W CARBON LINEAR</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>7.16</v>
+        <v>1.46</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1439,22 +1491,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1570-MR3010E12B1+6-RSR-ND</t>
+          <t>1738-1038-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MR3010E12B1+6-RSR</t>
+          <t>DFR0229</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FAN AXIAL 30X10MM 12VDC WIRE</t>
+          <t>MICROSD CARD MODULE FOR ARDUINO</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>25.2</v>
+        <v>7.16</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -1466,6 +1518,81 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1570-MR3010E12B1+6-RSR-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>MR3010E12B1+6-RSR</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>FAN AXIAL 30X10MM 12VDC WIRE</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1564,13 +1691,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1610,570 +1737,18 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>PEC11R-4220F-S0024-ND</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>PEC11R-4220F-S0024</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ROTARY ENCODER MECHANICAL 24PPR</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>2.876</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1778-WPM467-ND</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>WPM467</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>BREADBOARD 3.3V/5V POWER SUPPLY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>11.03</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>SJ5003-0-ND</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>SJ-5003 (BLACK)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>BUMPER CYLINDRICAL 0.44" DIA BLK</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="n">
-        <v>0.17054</v>
-      </c>
-      <c r="F4" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>473-1000-ND</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>503</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>PROTO BOARD COPPER CLAD 5" X 3"</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="n">
-        <v>11.95</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>255-2102-5-ND</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>AQG22105</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>SSR RELAY SPST-NO 2A 75-264V</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="n">
-        <v>8.210000000000001</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>732-61300621821-ND</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>61300621821</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>WR-PHD 2.54 MM DUAL SOCKET HEADE</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="F7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>497-3278-5-ND</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>TYN1225RG</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>SCR 1.2KV 25A TO220AB</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>4.98</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>160-1374-5-ND</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>MOC3021</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>OPTOISOLATOR 5KV TRIAC 6DIP</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>0.84</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>1740-1017-ND</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>BT136-600D,127</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>TRIAC SENS GATE 600V 4A TO220AB</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>DF02MDI-ND</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>DF02M</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>BRIDGE RECT 1PHASE 200KV 1A DFM</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="F11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2223-TS02-66-70-BK-160-LCR-D-ND</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>TS02-66-70-BK-160-LCR-D</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>6 X 6 MM, 7 MM ACTUATOR HEIGHT,</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>0.1404</v>
-      </c>
-      <c r="F12" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>732-61300821821-ND</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>61300821821</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>WR-PHD 2.54 MM DUAL SOCKET HEADE</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F13" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2057-RS2-04-G-ND</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>RS2-04-G</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>RECEPTACLE STRIP 4P 2.54MM PITCH</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.495</v>
-      </c>
-      <c r="F14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>2057-RS1-04-G-ND</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>RS1-04-G</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>RECEPTACLE STRIP 4P 2.54MM PITCH</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>0.384</v>
-      </c>
-      <c r="F15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2151-AS-16.000-18-ND</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>AS-16.000-18</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>CRYSTAL 16.0000MHZ 18PF TH</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>0.192</v>
-      </c>
-      <c r="F16" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>BAT-HLD-001-THM-ND</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>BAT-HLD-001-THM</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>BATT RETAIN COIN 1 CELL PC PIN</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="n">
-        <v>0.551</v>
-      </c>
-      <c r="F17" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>501-2446-ND</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>3781-48-0</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>MINI HOOK TO MINI HOOK 48"</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="F18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>501-2447-ND</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3781-48-2</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MINI HOOK TO MINI HOOK 48"</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>3781-48-9-ND</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>3781-48-9</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>MINI HOOK TO MINI HOOK 48"</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="F20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>501-1978-ND</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>3781-48-5</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>MINI HOOK TO MINI HOOK 48"</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="n">
-        <v>10.3</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>473-1048-ND</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>855-5</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>BRUSH SGL HEAD HORSE HAIR 6" 5PC</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="n">
-        <v>10.46</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>16-35792-ND</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>35792</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>YELLOW WASH BOTTLE, 8 OZ, DURAST</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="n">
-        <v>19.67</v>
-      </c>
-      <c r="F23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>315-NC191LTA10-ND</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>NC191LTA10</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>SMOOTH FLOW LOW TEMP SOLDER PAST</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="n">
-        <v>11.39</v>
-      </c>
-      <c r="F24" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2216,49 +1791,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DKS-PCB-RULER-ND</t>
+          <t>2151-AS-16.000-18-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DKS-PCB-RULER-12INCH</t>
+          <t>AS-16.000-18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PCB LAYOUT REFERENCE RULER 12"</t>
+          <t>CRYSTAL 16.0000MHZ 18PF TH</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>7.26</v>
+        <v>0.192</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1568-1600-ND</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>COM-10001</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>KNOB KNURLED 0.236" METAL</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="n">
-        <v>2.45</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2315,54 +1866,567 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>399-C0805C103K1RAC7800CT-ND</t>
+          <t>399-C0805C220J5GAC7210CT-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C0805C103K1RAC7800</t>
+          <t>C0805C220J5GAC7210</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CAP CER 10000PF 100V X7R 0805</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>10NF OR 0.01UF</t>
-        </is>
-      </c>
+          <t>CAP CER 22PF 50V C0G/NP0 0805</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.081</v>
+        <v>0.0414</v>
       </c>
       <c r="F2" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>490-16824-1-ND</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GRM21BR61E106KA73K</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CAP CER 10UF 25V X5R 0805</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>0.1008</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>478-3057-1-ND</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TAJR475M010RNJ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CAP TANT 4.7UF 20% 10V 0805</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1276-2891-1-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CL21A106KAYNNNE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CAP CER 10UF 25V X5R 0805</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="F5" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1276-CL21A226MAYNNNECT-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CL21A226MAYNNNE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CAP CER 22UF 25V X5R 0805</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.1646</v>
+      </c>
+      <c r="F6" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1276-1043-1-ND</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CL05A104KA5NNNC</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CAP CER 0.1UF 25V X5R 0402</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="F7" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>490-GCM0335C1E220JA16DCT-ND</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>GCM0335C1E220JA16D</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CAP CER 22PF 25V C0G/NP0 0201</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>0.0196</v>
+      </c>
+      <c r="F8" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>490-GRM0335C1H220FA01DCT-ND</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GRM0335C1H220FA01D</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CAP CER 22PF 50V C0G/NP0 0201</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.0236</v>
+      </c>
+      <c r="F9" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>399-C0805C103K1RAC7800CT-ND</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C0805C103K1RAC7800</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CAP CER 10000PF 100V X7R 0805</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>10NF OR 0.01UF</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="F10" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
           <t>399-C0805C104K5RAC7800CT-ND</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C0805C104K5RAC7800</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CAP CER 0.1UF 50V X7R 0805</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>100NF OR 0.1UF</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="F11" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>P16560CT-ND</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>35SVPF22M</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CAP ALUM POLY 22UF 20% 35V SMD</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="F12" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>399-A768MS107M1HLAE024CT-ND</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>A768MS107M1HLAE024</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CAP ALUM POLY 100UF 20% 50V SMD</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1276-1002-1-ND</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CL05B104KP5NNNC</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CAP CER 0.1UF 10V X7R 0402</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="F14" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>PEC11R-4220F-S0024-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PEC11R-4220F-S0024</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ROTARY ENCODER MECHANICAL 24PPR</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>2.876</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>255-2102-5-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AQG22105</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSR RELAY SPST-NO 2A 75-264V</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>8.210000000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Digi-Key Part #</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Manufacturer Part Number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Customer Reference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unit Price</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>732-12918-ND</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>971100244</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BRASS SPACER STUD METRIC THREAD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BAT-HLD-001-THM-ND</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C0805C104K5RAC7800</t>
+          <t>BAT-HLD-001-THM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CAP CER 0.1UF 50V X7R 0805</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>100NF OR 0.1UF</t>
-        </is>
-      </c>
+          <t>BATT RETAIN COIN 1 CELL PC PIN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.145</v>
+        <v>0.551</v>
       </c>
       <c r="F3" t="n">
         <v>20</v>
@@ -2371,265 +2435,361 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>P16560CT-ND</t>
+          <t>501-2446-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>35SVPF22M</t>
+          <t>3781-48-0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CAP ALUM POLY 22UF 20% 35V SMD</t>
+          <t>MINI HOOK TO MINI HOOK 48"</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>1.94</v>
+        <v>10.3</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>399-A768MS107M1HLAE024CT-ND</t>
+          <t>501-2447-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>A768MS107M1HLAE024</t>
+          <t>3781-48-2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CAP ALUM POLY 100UF 20% 50V SMD</t>
+          <t>MINI HOOK TO MINI HOOK 48"</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>1.36</v>
+        <v>10.3</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1276-1002-1-ND</t>
+          <t>3781-48-9-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CL05B104KP5NNNC</t>
+          <t>3781-48-9</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CAP CER 0.1UF 10V X7R 0402</t>
+          <t>MINI HOOK TO MINI HOOK 48"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>0.0154</v>
+        <v>10.3</v>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1276-2891-1-ND</t>
+          <t>501-1978-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CL21A106KAYNNNE</t>
+          <t>3781-48-5</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CAP CER 10UF 25V X5R 0805</t>
+          <t>MINI HOOK TO MINI HOOK 48"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.102</v>
+        <v>10.3</v>
       </c>
       <c r="F7" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1276-CL21A226MAYNNNECT-ND</t>
+          <t>473-1048-ND</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CL21A226MAYNNNE</t>
+          <t>855-5</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CAP CER 22UF 25V X5R 0805</t>
+          <t>BRUSH SGL HEAD HORSE HAIR 6" 5PC</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.1646</v>
+        <v>10.46</v>
       </c>
       <c r="F8" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1276-1043-1-ND</t>
+          <t>16-35792-ND</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CL05A104KA5NNNC</t>
+          <t>35792</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CAP CER 0.1UF 25V X5R 0402</t>
+          <t>YELLOW WASH BOTTLE, 8 OZ, DURAST</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.0065</v>
+        <v>19.67</v>
       </c>
       <c r="F9" t="n">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>490-GCM0335C1E220JA16DCT-ND</t>
+          <t>315-NC191LTA10-ND</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>GCM0335C1E220JA16D</t>
+          <t>NC191LTA10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CAP CER 22PF 25V C0G/NP0 0201</t>
+          <t>SMOOTH FLOW LOW TEMP SOLDER PAST</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>0.0196</v>
+        <v>11.39</v>
       </c>
       <c r="F10" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>490-GRM0335C1H220FA01DCT-ND</t>
+          <t>1778-WPM467-ND</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>GRM0335C1H220FA01D</t>
+          <t>WPM467</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CAP CER 22PF 50V C0G/NP0 0201</t>
+          <t>BREADBOARD 3.3V/5V POWER SUPPLY</t>
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
-        <v>0.0236</v>
+        <v>11.03</v>
       </c>
       <c r="F11" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>399-C0805C220J5GAC7210CT-ND</t>
+          <t>SJ5003-0-ND</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>C0805C220J5GAC7210</t>
+          <t>SJ-5003 (BLACK)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CAP CER 22PF 50V C0G/NP0 0805</t>
+          <t>BUMPER CYLINDRICAL 0.44" DIA BLK</t>
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.0414</v>
+        <v>0.17054</v>
       </c>
       <c r="F12" t="n">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>490-16824-1-ND</t>
+          <t>497-3278-5-ND</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>GRM21BR61E106KA73K</t>
+          <t>TYN1225RG</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CAP CER 10UF 25V X5R 0805</t>
+          <t>SCR 1.2KV 25A TO220AB</t>
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
       <c r="E13" t="n">
-        <v>0.1008</v>
+        <v>4.98</v>
       </c>
       <c r="F13" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>478-3057-1-ND</t>
+          <t>160-1374-5-ND</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TAJR475M010RNJ</t>
+          <t>MOC3021</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CAP TANT 4.7UF 20% 10V 0805</t>
+          <t>OPTOISOLATOR 5KV TRIAC 6DIP</t>
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>0.43</v>
+        <v>0.84</v>
       </c>
       <c r="F14" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1740-1017-ND</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BT136-600D,127</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>TRIAC SENS GATE 600V 4A TO220AB</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>DF02MDI-ND</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>DF02M</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>BRIDGE RECT 1PHASE 200KV 1A DFM</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>DKS-PCB-RULER-ND</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>DKS-PCB-RULER-12INCH</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PCB LAYOUT REFERENCE RULER 12"</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1568-1600-ND</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>COM-10001</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>KNOB KNURLED 0.236" METAL</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2718,7 +2878,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2761,97 +2921,121 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1514-PN2222APBFREE-ND</t>
+          <t>MMBT2222ATPMSCT-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>PN2222A PBFREE</t>
+          <t>MMBT2222A-TP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TRANS NPN 40V 0.8A TO92-3</t>
+          <t>TRANS NPN 40V 0.6A SOT23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.67</v>
+        <v>0.0583</v>
       </c>
       <c r="F2" t="n">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PZT2222AT1GOSCT-ND</t>
+          <t>160-1366-5-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PZT2222AT1G</t>
+          <t>LTV-817</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TRANS NPN 40V 0.6A SOT223</t>
+          <t>OPTOISOLATR 5KV TRANSISTOR 4-DIP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.64</v>
+        <v>0.58</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>497-5236-1-ND</t>
+          <t>1514-PN2222APBFREE-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2STD1665T4</t>
+          <t>PN2222A PBFREE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TRANS NPN 65V 6A DPAK</t>
+          <t>TRANS NPN 40V 0.8A TO92-3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>1.54</v>
+        <v>0.67</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>160-1366-5-ND</t>
+          <t>PZT2222AT1GOSCT-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LTV-817</t>
+          <t>PZT2222AT1G</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>OPTOISOLATR 5KV TRANSISTOR 4-DIP</t>
+          <t>TRANS NPN 40V 0.6A SOT223</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.58</v>
+        <v>0.64</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>497-5236-1-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2STD1665T4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TRANS NPN 65V 6A DPAK</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2908,118 +3092,118 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SB5100DICT-ND</t>
+          <t>1727-3862-1-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SB5100-T</t>
+          <t>PMEG2020EH,115</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DIODE SCHOTTKY 100V 5A DO201AD</t>
+          <t>DIODE SCHOTTKY 20V 2A SOD123F</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>0.899</v>
+        <v>0.508</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SK54B-LTPMSCT-ND</t>
+          <t>CUS08F30H3FCT-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SK54B-LTP</t>
+          <t>CUS08F30,H3F</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DIODE SCHOTTKY 40V 5A DO214AA</t>
+          <t>DIODE SCHOTTKY 30V 800MA USC</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.7</v>
+        <v>0.318</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FDLL4148CT-ND</t>
+          <t>SB5100DICT-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>FDLL4148</t>
+          <t>SB5100-T</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>DIODE GEN PURP 100V 200MA SOD80</t>
+          <t>DIODE SCHOTTKY 100V 5A DO201AD</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.143</v>
+        <v>0.899</v>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1655-DSS14UCT-ND</t>
+          <t>SK54B-LTPMSCT-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DSS14U</t>
+          <t>SK54B-LTP</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>DIODE SCHOTTKY 40V 1A SOD123FL</t>
+          <t>DIODE SCHOTTKY 40V 5A DO214AA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.263</v>
+        <v>0.7</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1727-3862-1-ND</t>
+          <t>FDLL4148CT-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>PMEG2020EH,115</t>
+          <t>FDLL4148</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DIODE SCHOTTKY 20V 2A SOD123F</t>
+          <t>DIODE GEN PURP 100V 200MA SOD80</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>0.508</v>
+        <v>0.143</v>
       </c>
       <c r="F6" t="n">
         <v>20</v>
@@ -3028,25 +3212,25 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CUS08F30H3FCT-ND</t>
+          <t>1655-DSS14UCT-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CUS08F30,H3F</t>
+          <t>DSS14U</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>DIODE SCHOTTKY 30V 800MA USC</t>
+          <t>DIODE SCHOTTKY 40V 1A SOD123FL</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.318</v>
+        <v>0.263</v>
       </c>
       <c r="F7" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -3060,7 +3244,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3151,288 +3335,96 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2057-ICS-308-T-ND</t>
+          <t>AZ1117IH-3.3TRG1DICT-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ICS-308-T</t>
+          <t>AZ1117IH-3.3TRG1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IC SOCKET, DIP, 8P 2.54MM PITCH</t>
+          <t>IC REG LINEAR 3.3V 1A SOT223</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.198</v>
+        <v>0.469</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TC74HC08APF-ND</t>
+          <t>788-1091-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TC74HC08APF</t>
+          <t>4006-020</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IC GATE AND 4CH 2-INP 14DIP</t>
+          <t>IC CURRENT REGULATOR MODULE</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>0.6899999999999999</v>
+        <v>3.97</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TC74HC14APF-ND</t>
+          <t>296-43515-5-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TC74HC14APF</t>
+          <t>LM2679S-ADJ/NOPB</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>IC INVERT SCHMITT 6CH 1-IN 14DIP</t>
+          <t>IC REG BUCK ADJ 5A TO263-7</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>0.71</v>
+        <v>11.01</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TC74HC00APF-ND</t>
+          <t>AS78L05RTR-G1DICT-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TC74HC00APF</t>
+          <t>AS78L05RTR-G1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IC GATE NAND 4CH 2-INP 14DIP</t>
+          <t>IC REG LINEAR 5V 100MA SOT89-3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.74</v>
+        <v>0.505</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>296-2028-ND</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>CD4001BE</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>IC GATE NOR 4CH 2-INP 14DIP</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>0.8100000000000001</v>
-      </c>
-      <c r="F8" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>296-12803-5-ND</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>CD74HC32E</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>IC GATE OR 4CH 2-INP 14DIP</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="F9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>296-8294-5-ND</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>SN74HC266N</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>IC GATE XNOR OD 4CH 2-INP 14DIP</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="n">
-        <v>1.03</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>296-14128-ND</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>CD4070BE</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>IC GATE XOR 4CH 2-INP 14DIP</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F11" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>AZ1117IH-3.3TRG1DICT-ND</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>AZ1117IH-3.3TRG1</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>IC REG LINEAR 3.3V 1A SOT223</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>0.469</v>
-      </c>
-      <c r="F12" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ATTINY84A-PU-ND</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>ATTINY84A-PU</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>IC MCU 8BIT 8KB FLASH 14DIP</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>2.48</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ATMEGA328-PU-ND</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>ATMEGA328-PU</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>IC MCU 8BIT 32KB FLASH 28DIP</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>4.03</v>
-      </c>
-      <c r="F14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>296-1336-1-ND</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TLC555CDR</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>IC OSC SGL TIMER 2.1MHZ 8-SOIC</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>1.089</v>
-      </c>
-      <c r="F15" t="n">
         <v>10</v>
       </c>
     </row>
@@ -3447,7 +3439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3490,70 +3482,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>788-1091-ND</t>
+          <t>296-1336-1-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4006-020</t>
+          <t>TLC555CDR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>IC CURRENT REGULATOR MODULE</t>
+          <t>IC OSC SGL TIMER 2.1MHZ 8-SOIC</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>3.97</v>
+        <v>1.089</v>
       </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>296-1414-5-ND</t>
+          <t>2057-ICS-308-T-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RC4558P</t>
+          <t>ICS-308-T</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
+          <t>IC SOCKET, DIP, 8P 2.54MM PITCH</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>0.63</v>
+        <v>0.198</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>296-NE555P-ND</t>
+          <t>TC74HC14APF-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NE555P</t>
+          <t>TC74HC14APF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IC OSC SINGLE TIMER 100KHZ 8-DIP</t>
+          <t>IC INVERT SCHMITT 6CH 1-IN 14DIP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.59</v>
+        <v>0.71</v>
       </c>
       <c r="F4" t="n">
         <v>5</v>
@@ -3562,289 +3554,145 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>296-43515-5-ND</t>
+          <t>ATTINY84A-PU-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LM2679S-ADJ/NOPB</t>
+          <t>ATTINY84A-PU</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IC REG BUCK ADJ 5A TO263-7</t>
+          <t>IC MCU 8BIT 8KB FLASH 14DIP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>11.01</v>
+        <v>2.48</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>296-14118-5-ND</t>
+          <t>ATMEGA328-PU-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CD4056BE</t>
+          <t>ATMEGA328-PU</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>IC DRVR 7 SEGMENT 1 DIGIT 16DIP</t>
+          <t>IC MCU 8BIT 32KB FLASH 28DIP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>1.02</v>
+        <v>4.03</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>296-31512-1-ND</t>
+          <t>296-1414-5-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CD4056BM96</t>
+          <t>RC4558P</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IC DRVR 7 SEGMENT 1 DIGIT 16SOIC</t>
+          <t>IC OPAMP GP 2 CIRCUIT 8DIP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.8</v>
+        <v>0.63</v>
       </c>
       <c r="F7" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AS78L05RTR-G1DICT-ND</t>
+          <t>296-NE555P-ND</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AS78L05RTR-G1</t>
+          <t>NE555P</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>IC REG LINEAR 5V 100MA SOT89-3</t>
+          <t>IC OSC SINGLE TIMER 100KHZ 8-DIP</t>
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
-        <v>0.505</v>
+        <v>0.59</v>
       </c>
       <c r="F8" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>277-12547-ND</t>
+          <t>296-14118-5-ND</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>5442206</t>
+          <t>CD4056BE</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>TERM BLK 2P SIDE ENT 5.08MM PCB</t>
+          <t>IC DRVR 7 SEGMENT 1 DIGIT 16DIP</t>
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.6850000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="F9" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>S7013-ND</t>
+          <t>296-31512-1-ND</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PPTC151LFBN-RC</t>
+          <t>CD4056BM96</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CONN HDR 15POS 0.1 TIN PCB</t>
+          <t>IC DRVR 7 SEGMENT 1 DIGIT 16SOIC</t>
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
       <c r="E10" t="n">
-        <v>1.203</v>
+        <v>0.8</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>455-2929-ND</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>SMR-03V-B</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>CONN RCPT HSG 3POS 2.50MM</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="n">
-        <v>0.183</v>
-      </c>
-      <c r="F11" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2073-USB4125-GF-ACT-ND</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>USB4125-GF-A</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>CONN RCPT TYPE C 6P SMD RA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="n">
-        <v>0.843</v>
-      </c>
-      <c r="F12" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>CP-102AH-ND</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>PJ-102AH</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>CONN PWR JACK 2X5.5MM SOLDER</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="F13" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2057-PH2-06-UA-ND</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>PH2-06-UA</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CONN HEADER VERT 6POS 2.54MM</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="n">
-        <v>0.144</v>
-      </c>
-      <c r="F14" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>S7018-ND</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>PPTC201LFBN-RC</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>CONN HDR 20POS 0.1 TIN PCB</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="n">
-        <v>1.511</v>
-      </c>
-      <c r="F15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>2073-USB4110-GF-A-1-ND</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>USB4110-GF-A</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>CONN RCP USB2.0 TYP C 24P SMD RA</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="n">
-        <v>1.638</v>
-      </c>
-      <c r="F16" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3858,7 +3706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3901,193 +3749,145 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A98333-ND</t>
+          <t>TC74HC08APF-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>282834-2</t>
+          <t>TC74HC08APF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TERM BLK 2P SIDE ENT 2.54MM PCB</t>
+          <t>IC GATE AND 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>2.01</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ED10563-ND</t>
+          <t>TC74HC00APF-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OSTVN04A150</t>
+          <t>TC74HC00APF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>TERM BLK 4P SIDE ENT 2.54MM PCB</t>
+          <t>IC GATE NAND 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>2.01</v>
+        <v>0.74</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2092-SX1100-B-ND</t>
+          <t>296-2028-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SX1100-B</t>
+          <t>CD4001BE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CONN SHUNT BLACK OPEN TOP</t>
+          <t>IC GATE NOR 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.078</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GC399-ND</t>
+          <t>296-12803-5-ND</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>33-1402</t>
+          <t>CD74HC32E</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CONN BARRIER SPKR STRIP 2CIRCUIT</t>
+          <t>IC GATE OR 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>3.54</v>
+        <v>0.75</v>
       </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A98077-ND</t>
+          <t>296-8294-5-ND</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>282836-3</t>
+          <t>SN74HC266N</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>TERM BLK 3POS SIDE ENTRY 5MM PCB</t>
+          <t>IC GATE XNOR OD 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>1.85</v>
+        <v>1.03</v>
       </c>
       <c r="F6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>455-2271-ND</t>
+          <t>296-14128-ND</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B6B-XH-A(LF)(SN)</t>
+          <t>CD4070BE</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CONN HEADER VERT 6POS 2.5MM</t>
+          <t>IC GATE XOR 4CH 2-INP 14DIP</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="n">
-        <v>0.367</v>
+        <v>0.78</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>455-2218-ND</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>XHP-6</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CONN RCPT HSG 6POS 2.50MM</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="n">
-        <v>0.182</v>
-      </c>
-      <c r="F8" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>455-2261-1-ND</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SXH-002T-P0.6</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>CONN SOCKET 26-30AWG CRIMP TIN</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="n">
-        <v>0.0546</v>
-      </c>
-      <c r="F9" t="n">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -4101,7 +3901,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4144,73 +3944,529 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1830-1161-ND</t>
+          <t>609-4618-1-ND</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>INND-TS56RCB</t>
+          <t>10118194-0001LF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>DISPLAY 7SEG 0.56" SGL RED 10DIP</t>
+          <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>1.73</v>
+        <v>0.579</v>
       </c>
       <c r="F2" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EG1903-ND</t>
+          <t>CP-002AHPJCT-ND</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EG1218</t>
+          <t>PJ-002AH-SMT-TR</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SWITCH SLIDE SPDT 200MA 30V</t>
+          <t>CONN PWR JACK 2X5.5MM SOLDER</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>1.04</v>
+        <v>2.09</v>
       </c>
       <c r="F3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CT2104MS-ND</t>
+          <t>S7018-ND</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>210-4MS</t>
+          <t>PPTC201LFBN-RC</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SWITCH SLIDE DIP SPST 100MA 20V</t>
+          <t>CONN HDR 20POS 0.1 TIN PCB</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="n">
-        <v>0.72</v>
+        <v>1.511</v>
       </c>
       <c r="F4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2073-USB4110-GF-A-1-ND</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>USB4110-GF-A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CONN RCP USB2.0 TYP C 24P SMD RA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
+        <v>1.638</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>277-12547-ND</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>5442206</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>TERM BLK 2P SIDE ENT 5.08MM PCB</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
+        <v>0.6850000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>732-61300621821-ND</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>61300621821</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>WR-PHD 2.54 MM DUAL SOCKET HEADE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>S7013-ND</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PPTC151LFBN-RC</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CONN HDR 15POS 0.1 TIN PCB</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
+        <v>1.203</v>
+      </c>
+      <c r="F8" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>455-2929-ND</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>SMR-03V-B</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CONN RCPT HSG 3POS 2.50MM</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
+        <v>0.183</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2073-USB4125-GF-ACT-ND</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>USB4125-GF-A</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CONN RCPT TYPE C 6P SMD RA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>0.843</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CP-102AH-ND</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PJ-102AH</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CONN PWR JACK 2X5.5MM SOLDER</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="F11" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2057-PH2-06-UA-ND</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PH2-06-UA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CONN HEADER VERT 6POS 2.54MM</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>0.144</v>
+      </c>
+      <c r="F12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>732-61300821821-ND</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>61300821821</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>WR-PHD 2.54 MM DUAL SOCKET HEADE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="F13" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2057-RS2-04-G-ND</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>RS2-04-G</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>RECEPTACLE STRIP 4P 2.54MM PITCH</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="n">
+        <v>0.495</v>
+      </c>
+      <c r="F14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2057-RS1-04-G-ND</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>RS1-04-G</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>RECEPTACLE STRIP 4P 2.54MM PITCH</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
+        <v>0.384</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>A98333-ND</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>282834-2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>TERM BLK 2P SIDE ENT 2.54MM PCB</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="F16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ED10563-ND</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>OSTVN04A150</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>TERM BLK 4P SIDE ENT 2.54MM PCB</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="n">
+        <v>2.01</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2092-SX1100-B-ND</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SX1100-B</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>CONN SHUNT BLACK OPEN TOP</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>GC399-ND</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>33-1402</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>CONN BARRIER SPKR STRIP 2CIRCUIT</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>3.54</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>A98077-ND</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>282836-3</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>TERM BLK 3POS SIDE ENTRY 5MM PCB</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>455-2271-ND</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>B6B-XH-A(LF)(SN)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>CONN HEADER VERT 6POS 2.5MM</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="n">
+        <v>0.367</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>455-2218-ND</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>XHP-6</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>CONN RCPT HSG 6POS 2.50MM</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>0.182</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>455-2261-1-ND</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SXH-002T-P0.6</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CONN SOCKET 26-30AWG CRIMP TIN</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="F23" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>